<commit_message>
Commited changes for Fluent wait and RowNumber in data drivern
</commit_message>
<xml_diff>
--- a/UploadData/NewApp.xlsx
+++ b/UploadData/NewApp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>DOTNumber</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Equipment &amp; Driver List.xlsx</t>
+  </si>
+  <si>
+    <t>RowNumber</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -526,285 +529,308 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>23</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>26</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>27</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>34</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>37</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>39</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>40</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>43</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>47</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>48</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>49</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>50</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>51</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>52</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>53</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>54</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>505638</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
-      </c>
-      <c r="F2">
-        <v>50</v>
       </c>
       <c r="G2">
         <v>50</v>
       </c>
-      <c r="J2" t="s">
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="K2" t="s">
         <v>58</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="L2">
-        <v>50</v>
-      </c>
       <c r="M2">
-        <v>50</v>
-      </c>
-      <c r="T2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2">
+        <v>25</v>
+      </c>
+      <c r="O2">
+        <v>25</v>
+      </c>
+      <c r="P2">
+        <v>25</v>
+      </c>
+      <c r="U2" t="s">
         <v>24</v>
       </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
       <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
         <v>1042</v>
       </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
       <c r="X2">
         <v>1</v>
       </c>
       <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
         <v>3042</v>
       </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
       <c r="AA2">
         <v>1</v>
       </c>
       <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
         <v>3213</v>
       </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
       <c r="AD2">
         <v>1</v>
       </c>
       <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
         <v>4123</v>
       </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="s">
         <v>38</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>41</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>42</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>44</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>46</v>
       </c>
-      <c r="AL2">
-        <v>1</v>
-      </c>
-      <c r="AM2" t="b">
+      <c r="AM2">
         <v>1</v>
       </c>
       <c r="AN2" t="b">
         <v>1</v>
       </c>
-      <c r="AR2" t="s">
-        <v>55</v>
+      <c r="AO2" t="b">
+        <v>1</v>
       </c>
       <c r="AS2" t="s">
         <v>55</v>
       </c>
       <c r="AT2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU2" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commited changes for Temp xml
</commit_message>
<xml_diff>
--- a/UploadData/NewApp.xlsx
+++ b/UploadData/NewApp.xlsx
@@ -524,7 +524,7 @@
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,16 +750,10 @@
         <v>14</v>
       </c>
       <c r="M2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="N2">
-        <v>25</v>
-      </c>
-      <c r="O2">
-        <v>25</v>
-      </c>
-      <c r="P2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="U2" t="s">
         <v>24</v>

</xml_diff>